<commit_message>
CV Power BI template
</commit_message>
<xml_diff>
--- a/experience.xlsx
+++ b/experience.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\cv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\CV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074F735D-7D50-4637-B960-0B8B2F228865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F64F074-234C-4F16-82F5-919A10B18775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="1944" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>school</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Przygotowanie do egzaminu ósmoklasisty i matury, Nadrabianie zaległości.</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>Self-emplyment</t>
   </si>
 </sst>
 </file>
@@ -483,19 +489,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.21875" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,8 +512,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -516,8 +526,11 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -527,8 +540,11 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -537,6 +553,9 @@
       </c>
       <c r="C4" t="s">
         <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -546,15 +565,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336099DC-9C7C-4235-9976-EE1E7CD738E3}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -567,8 +586,11 @@
       <c r="D1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -581,8 +603,11 @@
       <c r="D2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -595,16 +620,25 @@
       <c r="D3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -614,15 +648,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACA1065-A29A-4F5D-AD8D-9AA1BB43D0F3}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -632,8 +666,11 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -643,8 +680,11 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -654,8 +694,11 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -664,6 +707,9 @@
       </c>
       <c r="C4" t="s">
         <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -673,15 +719,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD118B78-F1A5-40C7-80EE-5106B3098B5A}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -694,8 +740,11 @@
       <c r="D1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -708,8 +757,11 @@
       <c r="D2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -722,8 +774,11 @@
       <c r="D3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -732,6 +787,9 @@
       </c>
       <c r="D4" t="s">
         <v>45</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>